<commit_message>
add force mode to fb_retain
</commit_message>
<xml_diff>
--- a/MIC7001/说明书/MIC7001-A3端口说明.V5.202012.1.xlsx
+++ b/MIC7001/说明书/MIC7001-A3端口说明.V5.202012.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28110" windowHeight="13140" activeTab="1"/>
+    <workbookView windowWidth="28125" windowHeight="12540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="按端子号排序" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="397">
   <si>
     <t>IMC7001-A3 插座C（左）V5.191031</t>
   </si>
@@ -1182,6 +1182,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>上面标记</t>
     </r>
     <r>
@@ -1305,6 +1312,12 @@
     <t>定制型号MIC7001-A3R： PWM4~11的内部对地器件由续流二极管改为2K电阻，用于电压型比例阀调节</t>
   </si>
   <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>定制型号MIC7001-A3C: D端口所有高有效DO/PWM输出端口无效</t>
+  </si>
+  <si>
     <t>DO编号</t>
   </si>
   <si>
@@ -1520,10 +1533,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1586,37 +1599,24 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1631,7 +1631,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1639,7 +1654,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1654,14 +1677,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -1669,16 +1684,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1692,24 +1721,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1722,14 +1743,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -1737,7 +1750,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1782,6 +1795,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1800,7 +1819,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1812,19 +1837,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1842,19 +1879,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1866,109 +1981,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2084,15 +2103,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2104,6 +2114,54 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2134,45 +2192,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -2186,152 +2205,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2416,6 +2435,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2425,6 +2447,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2449,8 +2474,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2493,14 +2518,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -5563,1693 +5588,1693 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.35833333333333" style="41" customWidth="1"/>
-    <col min="2" max="2" width="4.55833333333333" style="41" customWidth="1"/>
-    <col min="3" max="3" width="7.16666666666667" style="41" customWidth="1"/>
-    <col min="4" max="4" width="7.39166666666667" style="41" customWidth="1"/>
-    <col min="5" max="5" width="6.40833333333333" style="41" customWidth="1"/>
-    <col min="6" max="6" width="6.625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="7.05833333333333" style="41" customWidth="1"/>
-    <col min="8" max="8" width="8.69166666666667" style="41" customWidth="1"/>
-    <col min="9" max="9" width="9.34166666666667" style="41" customWidth="1"/>
-    <col min="10" max="10" width="9" style="41"/>
-    <col min="11" max="11" width="10.7333333333333" style="41" customWidth="1"/>
-    <col min="12" max="12" width="5.20833333333333" style="41" customWidth="1"/>
-    <col min="13" max="13" width="4.89166666666667" style="41" customWidth="1"/>
-    <col min="14" max="14" width="8.04166666666667" style="41" customWidth="1"/>
-    <col min="15" max="15" width="6.95" style="41" customWidth="1"/>
-    <col min="16" max="16" width="6.08333333333333" style="41" customWidth="1"/>
-    <col min="17" max="17" width="6.625" style="41" customWidth="1"/>
-    <col min="18" max="18" width="7.38333333333333" style="41" customWidth="1"/>
-    <col min="19" max="19" width="8.69166666666667" style="41" customWidth="1"/>
-    <col min="20" max="20" width="8.25833333333333" style="41" customWidth="1"/>
-    <col min="21" max="21" width="7.825" style="41" customWidth="1"/>
-    <col min="22" max="22" width="10.5833333333333" style="41" customWidth="1"/>
-    <col min="23" max="23" width="9" style="41"/>
-    <col min="24" max="24" width="5.975" style="41" customWidth="1"/>
-    <col min="25" max="16384" width="9" style="41"/>
+    <col min="1" max="1" width="3.35833333333333" style="43" customWidth="1"/>
+    <col min="2" max="2" width="4.55833333333333" style="43" customWidth="1"/>
+    <col min="3" max="3" width="7.16666666666667" style="43" customWidth="1"/>
+    <col min="4" max="4" width="7.39166666666667" style="43" customWidth="1"/>
+    <col min="5" max="5" width="6.40833333333333" style="43" customWidth="1"/>
+    <col min="6" max="6" width="6.625" style="43" customWidth="1"/>
+    <col min="7" max="7" width="7.05833333333333" style="43" customWidth="1"/>
+    <col min="8" max="8" width="8.69166666666667" style="43" customWidth="1"/>
+    <col min="9" max="9" width="9.34166666666667" style="43" customWidth="1"/>
+    <col min="10" max="10" width="9" style="43"/>
+    <col min="11" max="11" width="10.7333333333333" style="43" customWidth="1"/>
+    <col min="12" max="12" width="5.20833333333333" style="43" customWidth="1"/>
+    <col min="13" max="13" width="4.89166666666667" style="43" customWidth="1"/>
+    <col min="14" max="14" width="8.04166666666667" style="43" customWidth="1"/>
+    <col min="15" max="15" width="6.95" style="43" customWidth="1"/>
+    <col min="16" max="16" width="6.08333333333333" style="43" customWidth="1"/>
+    <col min="17" max="17" width="6.625" style="43" customWidth="1"/>
+    <col min="18" max="18" width="7.38333333333333" style="43" customWidth="1"/>
+    <col min="19" max="19" width="8.69166666666667" style="43" customWidth="1"/>
+    <col min="20" max="20" width="8.25833333333333" style="43" customWidth="1"/>
+    <col min="21" max="21" width="7.825" style="43" customWidth="1"/>
+    <col min="22" max="22" width="10.5833333333333" style="43" customWidth="1"/>
+    <col min="23" max="23" width="9" style="43"/>
+    <col min="24" max="24" width="5.975" style="43" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="43"/>
   </cols>
   <sheetData>
-    <row r="2" s="41" customFormat="1" spans="2:22">
-      <c r="B2" s="42" t="s">
+    <row r="2" s="43" customFormat="1" spans="2:22">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="M2" s="42" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="M2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-    </row>
-    <row r="3" s="41" customFormat="1" ht="24.75" spans="2:22">
-      <c r="B3" s="43" t="s">
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+    </row>
+    <row r="3" s="43" customFormat="1" ht="24.75" spans="2:22">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="44" t="s">
+      <c r="N3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="44" t="s">
+      <c r="O3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="44" t="s">
+      <c r="P3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="44" t="s">
+      <c r="Q3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="44" t="s">
+      <c r="R3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="45" t="s">
+      <c r="S3" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="44" t="s">
+      <c r="T3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="43" t="s">
+      <c r="U3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="43" t="s">
+      <c r="V3" s="45" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" s="41" customFormat="1" spans="2:22">
-      <c r="B4" s="46" t="s">
+    <row r="4" s="43" customFormat="1" spans="2:22">
+      <c r="B4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46" t="s">
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="M4" s="46" t="s">
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="M4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46" t="s">
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="V4" s="43" t="s">
+      <c r="V4" s="45" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" s="41" customFormat="1" spans="2:22">
-      <c r="B5" s="46" t="s">
+    <row r="5" s="43" customFormat="1" spans="2:22">
+      <c r="B5" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="46" t="s">
+      <c r="M5" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="46" t="s">
+      <c r="N5" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="46" t="s">
+      <c r="O5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46" t="s">
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="S5" s="46" t="s">
+      <c r="S5" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-    </row>
-    <row r="6" s="41" customFormat="1" spans="2:22">
-      <c r="B6" s="46" t="s">
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+    </row>
+    <row r="6" s="43" customFormat="1" spans="2:22">
+      <c r="B6" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46" t="s">
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="M6" s="46" t="s">
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="M6" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="46" t="s">
+      <c r="N6" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="46" t="s">
+      <c r="O6" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46" t="s">
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="46" t="s">
+      <c r="S6" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="46"/>
-      <c r="U6" s="46"/>
-      <c r="V6" s="46"/>
-    </row>
-    <row r="7" s="41" customFormat="1" spans="2:22">
-      <c r="B7" s="46" t="s">
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
+    </row>
+    <row r="7" s="43" customFormat="1" spans="2:22">
+      <c r="B7" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46" t="s">
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="M7" s="46" t="s">
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="M7" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="46" t="s">
+      <c r="N7" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46" t="s">
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="S7" s="46" t="s">
+      <c r="S7" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="T7" s="46"/>
-      <c r="U7" s="46"/>
-      <c r="V7" s="46"/>
-    </row>
-    <row r="8" s="41" customFormat="1" spans="2:22">
-      <c r="B8" s="46" t="s">
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+    </row>
+    <row r="8" s="43" customFormat="1" spans="2:22">
+      <c r="B8" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46" t="s">
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="M8" s="46" t="s">
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="M8" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="N8" s="46" t="s">
+      <c r="N8" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="O8" s="46" t="s">
+      <c r="O8" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46" t="s">
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="S8" s="46" t="s">
+      <c r="S8" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
-    </row>
-    <row r="9" s="41" customFormat="1" spans="2:22">
-      <c r="B9" s="46" t="s">
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+    </row>
+    <row r="9" s="43" customFormat="1" spans="2:22">
+      <c r="B9" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46" t="s">
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="M9" s="46" t="s">
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="M9" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
-      <c r="U9" s="46" t="s">
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="V9" s="43" t="s">
+      <c r="V9" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" s="41" customFormat="1" spans="2:22">
-      <c r="B10" s="46" t="s">
+    <row r="10" s="43" customFormat="1" spans="2:22">
+      <c r="B10" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="43" t="s">
+      <c r="K10" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="46" t="s">
+      <c r="M10" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="N10" s="46" t="s">
+      <c r="N10" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="O10" s="46" t="s">
+      <c r="O10" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46" t="s">
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="S10" s="46" t="s">
+      <c r="S10" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="T10" s="46"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="46"/>
-    </row>
-    <row r="11" s="41" customFormat="1" spans="2:22">
-      <c r="B11" s="46" t="s">
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+    </row>
+    <row r="11" s="43" customFormat="1" spans="2:22">
+      <c r="B11" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46" t="s">
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="M11" s="46" t="s">
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="M11" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="N11" s="46" t="s">
+      <c r="N11" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="O11" s="46" t="s">
+      <c r="O11" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46" t="s">
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="S11" s="46" t="s">
+      <c r="S11" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="46"/>
-    </row>
-    <row r="12" s="41" customFormat="1" spans="2:22">
-      <c r="B12" s="46" t="s">
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+    </row>
+    <row r="12" s="43" customFormat="1" spans="2:22">
+      <c r="B12" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46" t="s">
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="M12" s="46" t="s">
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="M12" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="N12" s="46" t="s">
+      <c r="N12" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="O12" s="46" t="s">
+      <c r="O12" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46" t="s">
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="S12" s="46" t="s">
+      <c r="S12" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
-      <c r="V12" s="46"/>
-    </row>
-    <row r="13" s="41" customFormat="1" spans="2:22">
-      <c r="B13" s="46" t="s">
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+    </row>
+    <row r="13" s="43" customFormat="1" spans="2:22">
+      <c r="B13" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46" t="s">
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="46" t="s">
+      <c r="H13" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="M13" s="46" t="s">
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="M13" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="46" t="s">
+      <c r="N13" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="O13" s="46" t="s">
+      <c r="O13" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46" t="s">
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="S13" s="46" t="s">
+      <c r="S13" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
-      <c r="V13" s="46"/>
-    </row>
-    <row r="14" s="41" customFormat="1" spans="2:22">
-      <c r="B14" s="46" t="s">
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+    </row>
+    <row r="14" s="43" customFormat="1" spans="2:22">
+      <c r="B14" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46" t="s">
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="H14" s="46" t="s">
+      <c r="H14" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="M14" s="46" t="s">
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="M14" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="N14" s="46"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="46"/>
-      <c r="T14" s="46"/>
-      <c r="U14" s="46" t="s">
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+      <c r="U14" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="V14" s="43" t="s">
+      <c r="V14" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" s="41" customFormat="1" spans="2:22">
-      <c r="B15" s="46" t="s">
+    <row r="15" s="43" customFormat="1" spans="2:22">
+      <c r="B15" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46" t="s">
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="43" t="s">
+      <c r="K15" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="46" t="s">
+      <c r="M15" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="N15" s="46" t="s">
+      <c r="N15" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="O15" s="46" t="s">
+      <c r="O15" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="P15" s="46"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="46" t="s">
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="S15" s="46" t="s">
+      <c r="S15" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="T15" s="46"/>
-      <c r="U15" s="46"/>
-      <c r="V15" s="46"/>
-    </row>
-    <row r="16" s="41" customFormat="1" spans="2:22">
-      <c r="B16" s="46" t="s">
+      <c r="T15" s="48"/>
+      <c r="U15" s="48"/>
+      <c r="V15" s="48"/>
+    </row>
+    <row r="16" s="43" customFormat="1" spans="2:22">
+      <c r="B16" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46" t="s">
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="M16" s="46" t="s">
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="M16" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="N16" s="46" t="s">
+      <c r="N16" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="O16" s="46" t="s">
+      <c r="O16" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="46" t="s">
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="S16" s="46" t="s">
+      <c r="S16" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="T16" s="46"/>
-      <c r="U16" s="46"/>
-      <c r="V16" s="43" t="s">
+      <c r="T16" s="48"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="45" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" s="41" customFormat="1" spans="2:22">
-      <c r="B17" s="46" t="s">
+    <row r="17" s="43" customFormat="1" spans="2:22">
+      <c r="B17" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46" t="s">
+      <c r="C17" s="48"/>
+      <c r="D17" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="M17" s="46" t="s">
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="M17" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="N17" s="46" t="s">
+      <c r="N17" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="O17" s="46" t="s">
+      <c r="O17" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46" t="s">
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="R17" s="46"/>
-      <c r="S17" s="46"/>
-      <c r="T17" s="46"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="46"/>
-    </row>
-    <row r="18" s="41" customFormat="1" spans="2:22">
-      <c r="B18" s="46" t="s">
+      <c r="R17" s="48"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+    </row>
+    <row r="18" s="43" customFormat="1" spans="2:22">
+      <c r="B18" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46" t="s">
+      <c r="C18" s="48"/>
+      <c r="D18" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="M18" s="46" t="s">
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="M18" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="N18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
-      <c r="S18" s="46"/>
-      <c r="T18" s="46"/>
-      <c r="U18" s="46" t="s">
+      <c r="N18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="V18" s="43" t="s">
+      <c r="V18" s="45" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" s="41" customFormat="1" spans="2:22">
-      <c r="B19" s="46" t="s">
+    <row r="19" s="43" customFormat="1" spans="2:22">
+      <c r="B19" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46" t="s">
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="M19" s="46" t="s">
+      <c r="M19" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="N19" s="46" t="s">
+      <c r="N19" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="O19" s="46" t="s">
+      <c r="O19" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="46"/>
-      <c r="S19" s="46"/>
-      <c r="T19" s="46"/>
-      <c r="V19" s="46" t="s">
+      <c r="P19" s="48"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="48"/>
+      <c r="S19" s="48"/>
+      <c r="T19" s="48"/>
+      <c r="V19" s="48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="20" s="41" customFormat="1" spans="2:22">
-      <c r="B20" s="46" t="s">
+    <row r="20" s="43" customFormat="1" spans="2:22">
+      <c r="B20" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46" t="s">
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="M20" s="46" t="s">
+      <c r="M20" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="N20" s="46" t="s">
+      <c r="N20" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="O20" s="46" t="s">
+      <c r="O20" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="R20" s="46"/>
-      <c r="S20" s="46"/>
-      <c r="T20" s="46"/>
-      <c r="U20" s="46"/>
-      <c r="V20" s="46" t="s">
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" s="41" customFormat="1" spans="2:22">
-      <c r="B21" s="46" t="s">
+    <row r="21" s="43" customFormat="1" spans="2:22">
+      <c r="B21" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="M21" s="46" t="s">
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="M21" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="N21" s="46" t="s">
+      <c r="N21" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="O21" s="46" t="s">
+      <c r="O21" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="P21" s="46"/>
-      <c r="Q21" s="46"/>
-      <c r="R21" s="46"/>
-      <c r="S21" s="46"/>
-      <c r="T21" s="46"/>
-      <c r="U21" s="46"/>
-      <c r="V21" s="46"/>
-    </row>
-    <row r="22" s="41" customFormat="1" spans="2:22">
-      <c r="B22" s="46" t="s">
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+    </row>
+    <row r="22" s="43" customFormat="1" spans="2:22">
+      <c r="B22" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="M22" s="46" t="s">
+      <c r="E22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="M22" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="N22" s="46" t="s">
+      <c r="N22" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="O22" s="46" t="s">
+      <c r="O22" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="P22" s="46"/>
-      <c r="Q22" s="46"/>
-      <c r="R22" s="46"/>
-      <c r="S22" s="46"/>
-      <c r="T22" s="46"/>
-      <c r="U22" s="46"/>
-      <c r="V22" s="46" t="s">
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" s="41" customFormat="1" spans="2:22">
-      <c r="B23" s="46" t="s">
+    <row r="23" s="43" customFormat="1" spans="2:22">
+      <c r="B23" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="M23" s="46" t="s">
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="M23" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="N23" s="46" t="s">
+      <c r="N23" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="O23" s="46" t="s">
+      <c r="O23" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="46"/>
-      <c r="V23" s="46" t="s">
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="48"/>
+      <c r="U23" s="48"/>
+      <c r="V23" s="48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="24" s="41" customFormat="1" spans="2:22">
-      <c r="B24" s="46" t="s">
+    <row r="24" s="43" customFormat="1" spans="2:22">
+      <c r="B24" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="C24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46" t="s">
+      <c r="C24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="K24" s="43" t="s">
+      <c r="K24" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="M24" s="46" t="s">
+      <c r="M24" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46" t="s">
+      <c r="N24" s="48"/>
+      <c r="O24" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="P24" s="46" t="s">
+      <c r="P24" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="46"/>
-      <c r="S24" s="46"/>
-      <c r="T24" s="46"/>
-      <c r="U24" s="46"/>
-      <c r="V24" s="46"/>
-    </row>
-    <row r="25" s="41" customFormat="1" spans="2:22">
-      <c r="B25" s="46" t="s">
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="48"/>
+      <c r="V24" s="48"/>
+    </row>
+    <row r="25" s="43" customFormat="1" spans="2:22">
+      <c r="B25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D25" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="F25" s="46" t="s">
+      <c r="F25" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="M25" s="46" t="s">
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="M25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46" t="s">
+      <c r="N25" s="48"/>
+      <c r="O25" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="P25" s="46" t="s">
+      <c r="P25" s="48" t="s">
         <v>156</v>
       </c>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="46"/>
-      <c r="T25" s="46"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="46"/>
-    </row>
-    <row r="26" s="41" customFormat="1" spans="2:22">
-      <c r="B26" s="46" t="s">
+      <c r="Q25" s="48"/>
+      <c r="R25" s="48"/>
+      <c r="S25" s="48"/>
+      <c r="T25" s="48"/>
+      <c r="U25" s="48"/>
+      <c r="V25" s="48"/>
+    </row>
+    <row r="26" s="43" customFormat="1" spans="2:22">
+      <c r="B26" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46" t="s">
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="H26" s="46" t="s">
+      <c r="H26" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="43" t="s">
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="M26" s="46" t="s">
+      <c r="M26" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="N26" s="46" t="s">
+      <c r="N26" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="O26" s="46" t="s">
+      <c r="O26" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="P26" s="46"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="46" t="s">
+      <c r="P26" s="48"/>
+      <c r="Q26" s="48"/>
+      <c r="R26" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="S26" s="46" t="s">
+      <c r="S26" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="T26" s="46"/>
-      <c r="U26" s="46"/>
-      <c r="V26" s="46"/>
-    </row>
-    <row r="27" s="41" customFormat="1" spans="2:22">
-      <c r="B27" s="46" t="s">
+      <c r="T26" s="48"/>
+      <c r="U26" s="48"/>
+      <c r="V26" s="48"/>
+    </row>
+    <row r="27" s="43" customFormat="1" spans="2:22">
+      <c r="B27" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46" t="s">
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="H27" s="46" t="s">
+      <c r="H27" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
-      <c r="M27" s="46" t="s">
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="M27" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="N27" s="46" t="s">
+      <c r="N27" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="O27" s="46" t="s">
+      <c r="O27" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="P27" s="46"/>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="46" t="s">
+      <c r="P27" s="48"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="S27" s="46" t="s">
+      <c r="S27" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="T27" s="46"/>
-      <c r="U27" s="46"/>
-      <c r="V27" s="43" t="s">
+      <c r="T27" s="48"/>
+      <c r="U27" s="48"/>
+      <c r="V27" s="45" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" s="41" customFormat="1" spans="2:22">
-      <c r="B28" s="46" t="s">
+    <row r="28" s="43" customFormat="1" spans="2:22">
+      <c r="B28" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46" t="s">
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="H28" s="46" t="s">
+      <c r="H28" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="I28" s="46"/>
-      <c r="J28" s="46"/>
-      <c r="K28" s="46"/>
-      <c r="M28" s="46" t="s">
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="M28" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="N28" s="46"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46" t="s">
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="S28" s="46" t="s">
+      <c r="S28" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="T28" s="46" t="s">
+      <c r="T28" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="U28" s="46"/>
-      <c r="V28" s="46"/>
-    </row>
-    <row r="29" s="41" customFormat="1" spans="2:22">
-      <c r="B29" s="46" t="s">
+      <c r="U28" s="48"/>
+      <c r="V28" s="48"/>
+    </row>
+    <row r="29" s="43" customFormat="1" spans="2:22">
+      <c r="B29" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46" t="s">
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="K29" s="43" t="s">
+      <c r="K29" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="M29" s="46" t="s">
+      <c r="M29" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46" t="s">
+      <c r="N29" s="48"/>
+      <c r="O29" s="48"/>
+      <c r="P29" s="48"/>
+      <c r="Q29" s="48"/>
+      <c r="R29" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="S29" s="46" t="s">
+      <c r="S29" s="48" t="s">
         <v>187</v>
       </c>
-      <c r="T29" s="46" t="s">
+      <c r="T29" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="U29" s="46"/>
-      <c r="V29" s="46"/>
-    </row>
-    <row r="30" s="41" customFormat="1" spans="2:22">
-      <c r="B30" s="46" t="s">
+      <c r="U29" s="48"/>
+      <c r="V29" s="48"/>
+    </row>
+    <row r="30" s="43" customFormat="1" spans="2:22">
+      <c r="B30" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46" t="s">
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="K30" s="43" t="s">
+      <c r="K30" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="M30" s="46" t="s">
+      <c r="M30" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="46"/>
-      <c r="S30" s="46"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="46" t="s">
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="48"/>
+      <c r="S30" s="48"/>
+      <c r="T30" s="48"/>
+      <c r="U30" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="V30" s="43" t="s">
+      <c r="V30" s="45" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" s="41" customFormat="1" spans="2:22">
-      <c r="B31" s="46" t="s">
+    <row r="31" s="43" customFormat="1" spans="2:22">
+      <c r="B31" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="48" t="s">
         <v>192</v>
       </c>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="43" t="s">
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="M31" s="46" t="s">
+      <c r="M31" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="N31" s="46" t="s">
+      <c r="N31" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="O31" s="46" t="s">
+      <c r="O31" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="46"/>
-      <c r="S31" s="46"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="46"/>
-      <c r="V31" s="46" t="s">
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="48"/>
+      <c r="V31" s="48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" s="41" customFormat="1" spans="2:22">
-      <c r="B32" s="46" t="s">
+    <row r="32" s="43" customFormat="1" spans="2:22">
+      <c r="B32" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="C32" s="46" t="s">
+      <c r="C32" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="M32" s="46" t="s">
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="M32" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="N32" s="46" t="s">
+      <c r="N32" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="O32" s="46" t="s">
+      <c r="O32" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="46"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="46"/>
-      <c r="V32" s="46" t="s">
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="48"/>
+      <c r="S32" s="48"/>
+      <c r="T32" s="48"/>
+      <c r="U32" s="48"/>
+      <c r="V32" s="48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="33" s="41" customFormat="1" spans="2:22">
-      <c r="B33" s="46" t="s">
+    <row r="33" s="43" customFormat="1" spans="2:22">
+      <c r="B33" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="M33" s="46" t="s">
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="M33" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="N33" s="46" t="s">
+      <c r="N33" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="O33" s="46" t="s">
+      <c r="O33" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="46"/>
-      <c r="V33" s="46" t="s">
+      <c r="P33" s="48"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="48"/>
+      <c r="S33" s="48"/>
+      <c r="T33" s="48"/>
+      <c r="U33" s="48"/>
+      <c r="V33" s="48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="34" s="41" customFormat="1" spans="2:22">
-      <c r="B34" s="46" t="s">
+    <row r="34" s="43" customFormat="1" spans="2:22">
+      <c r="B34" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
-      <c r="M34" s="46" t="s">
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="M34" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="N34" s="46" t="s">
+      <c r="N34" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="O34" s="46" t="s">
+      <c r="O34" s="48" t="s">
         <v>209</v>
       </c>
-      <c r="P34" s="46"/>
-      <c r="Q34" s="46"/>
-      <c r="R34" s="46"/>
-      <c r="S34" s="46"/>
-      <c r="T34" s="46"/>
-      <c r="U34" s="46"/>
-      <c r="V34" s="46" t="s">
+      <c r="P34" s="48"/>
+      <c r="Q34" s="48"/>
+      <c r="R34" s="48"/>
+      <c r="S34" s="48"/>
+      <c r="T34" s="48"/>
+      <c r="U34" s="48"/>
+      <c r="V34" s="48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="35" s="41" customFormat="1" spans="2:22">
-      <c r="B35" s="46" t="s">
+    <row r="35" s="43" customFormat="1" spans="2:22">
+      <c r="B35" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="46" t="s">
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="K35" s="43" t="s">
+      <c r="K35" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="M35" s="46" t="s">
+      <c r="M35" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="P35" s="46"/>
-      <c r="Q35" s="46"/>
-      <c r="R35" s="46"/>
-      <c r="S35" s="46"/>
-      <c r="T35" s="46"/>
-      <c r="U35" s="46" t="s">
+      <c r="P35" s="48"/>
+      <c r="Q35" s="48"/>
+      <c r="R35" s="48"/>
+      <c r="S35" s="48"/>
+      <c r="T35" s="48"/>
+      <c r="U35" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="V35" s="43" t="s">
+      <c r="V35" s="45" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="36" s="41" customFormat="1" spans="2:22">
-      <c r="B36" s="46" t="s">
+    <row r="36" s="43" customFormat="1" spans="2:22">
+      <c r="B36" s="48" t="s">
         <v>211</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46" t="s">
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="H36" s="46" t="s">
+      <c r="H36" s="48" t="s">
         <v>213</v>
       </c>
-      <c r="I36" s="46" t="s">
+      <c r="I36" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="J36" s="46"/>
-      <c r="K36" s="46"/>
-      <c r="M36" s="46" t="s">
+      <c r="J36" s="48"/>
+      <c r="K36" s="48"/>
+      <c r="M36" s="48" t="s">
         <v>211</v>
       </c>
-      <c r="N36" s="46"/>
-      <c r="O36" s="46"/>
-      <c r="P36" s="46"/>
-      <c r="Q36" s="46"/>
-      <c r="R36" s="46"/>
-      <c r="S36" s="46"/>
-      <c r="T36" s="46"/>
-      <c r="U36" s="46" t="s">
+      <c r="N36" s="48"/>
+      <c r="O36" s="48"/>
+      <c r="P36" s="48"/>
+      <c r="Q36" s="48"/>
+      <c r="R36" s="48"/>
+      <c r="S36" s="48"/>
+      <c r="T36" s="48"/>
+      <c r="U36" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="V36" s="43" t="s">
+      <c r="V36" s="45" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="37" s="41" customFormat="1" spans="2:22">
-      <c r="B37" s="46" t="s">
+    <row r="37" s="43" customFormat="1" spans="2:22">
+      <c r="B37" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46" t="s">
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48" t="s">
         <v>218</v>
       </c>
-      <c r="H37" s="46" t="s">
+      <c r="H37" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="I37" s="46" t="s">
+      <c r="I37" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="M37" s="46" t="s">
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="M37" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="N37" s="46" t="s">
+      <c r="N37" s="48" t="s">
         <v>221</v>
       </c>
-      <c r="O37" s="46" t="s">
+      <c r="O37" s="48" t="s">
         <v>222</v>
       </c>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46" t="s">
+      <c r="P37" s="48"/>
+      <c r="Q37" s="48"/>
+      <c r="R37" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="S37" s="46" t="s">
+      <c r="S37" s="48" t="s">
         <v>224</v>
       </c>
-      <c r="T37" s="46"/>
-      <c r="U37" s="46"/>
-      <c r="V37" s="46"/>
-    </row>
-    <row r="38" s="41" customFormat="1" spans="2:22">
-      <c r="B38" s="46" t="s">
+      <c r="T37" s="48"/>
+      <c r="U37" s="48"/>
+      <c r="V37" s="48"/>
+    </row>
+    <row r="38" s="43" customFormat="1" spans="2:22">
+      <c r="B38" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C38" s="48" t="s">
         <v>226</v>
       </c>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46" t="s">
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48" t="s">
         <v>228</v>
       </c>
-      <c r="H38" s="46" t="s">
+      <c r="H38" s="48" t="s">
         <v>229</v>
       </c>
-      <c r="I38" s="46"/>
-      <c r="J38" s="46"/>
-      <c r="K38" s="43" t="s">
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="M38" s="46" t="s">
+      <c r="M38" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="N38" s="46" t="s">
+      <c r="N38" s="48" t="s">
         <v>230</v>
       </c>
-      <c r="O38" s="46" t="s">
+      <c r="O38" s="48" t="s">
         <v>231</v>
       </c>
-      <c r="P38" s="46"/>
-      <c r="Q38" s="46"/>
-      <c r="R38" s="46" t="s">
+      <c r="P38" s="48"/>
+      <c r="Q38" s="48"/>
+      <c r="R38" s="48" t="s">
         <v>232</v>
       </c>
-      <c r="S38" s="46" t="s">
+      <c r="S38" s="48" t="s">
         <v>233</v>
       </c>
-      <c r="T38" s="46"/>
-      <c r="U38" s="46"/>
-      <c r="V38" s="46"/>
+      <c r="T38" s="48"/>
+      <c r="U38" s="48"/>
+      <c r="V38" s="48"/>
     </row>
     <row r="40" spans="3:3">
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="49" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="41" s="41" customFormat="1" spans="3:11">
-      <c r="C41" s="46" t="s">
+    <row r="41" s="43" customFormat="1" spans="3:11">
+      <c r="C41" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="48" t="s">
+      <c r="D41" s="50" t="s">
         <v>235</v>
       </c>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="J41" s="56"/>
-      <c r="K41" s="56"/>
-    </row>
-    <row r="42" s="41" customFormat="1" spans="3:11">
-      <c r="C42" s="46" t="s">
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="58"/>
+    </row>
+    <row r="42" s="43" customFormat="1" spans="3:11">
+      <c r="C42" s="48" t="s">
         <v>236</v>
       </c>
-      <c r="D42" s="49" t="s">
+      <c r="D42" s="51" t="s">
         <v>237</v>
       </c>
-      <c r="E42" s="49"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="J42" s="57"/>
-      <c r="K42" s="56"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="58"/>
     </row>
     <row r="43" spans="3:7">
-      <c r="C43" s="46" t="s">
+      <c r="C43" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="D43" s="49" t="s">
+      <c r="D43" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
     </row>
     <row r="44" spans="3:6">
-      <c r="C44" s="50"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
     </row>
     <row r="53" spans="3:3">
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="43" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="54" s="41" customFormat="1" spans="7:8">
-      <c r="G54" s="53" t="s">
+    <row r="54" s="43" customFormat="1" spans="7:8">
+      <c r="G54" s="55" t="s">
         <v>240</v>
       </c>
-      <c r="H54" s="53"/>
-    </row>
-    <row r="55" s="41" customFormat="1" spans="7:23">
-      <c r="G55" s="54" t="s">
+      <c r="H54" s="55"/>
+    </row>
+    <row r="55" s="43" customFormat="1" spans="7:23">
+      <c r="G55" s="56" t="s">
         <v>241</v>
       </c>
-      <c r="H55" s="55"/>
-      <c r="R55" s="54" t="s">
+      <c r="H55" s="57"/>
+      <c r="R55" s="56" t="s">
         <v>242</v>
       </c>
-      <c r="S55" s="55"/>
-      <c r="U55" s="54" t="s">
+      <c r="S55" s="57"/>
+      <c r="U55" s="56" t="s">
         <v>243</v>
       </c>
-      <c r="V55" s="58"/>
-      <c r="W55" s="55"/>
-    </row>
-    <row r="56" s="41" customFormat="1" spans="7:23">
-      <c r="G56" s="43" t="s">
+      <c r="V55" s="60"/>
+      <c r="W55" s="57"/>
+    </row>
+    <row r="56" s="43" customFormat="1" spans="7:23">
+      <c r="G56" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="H56" s="46"/>
-      <c r="R56" s="43" t="s">
+      <c r="H56" s="48"/>
+      <c r="R56" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="S56" s="46"/>
-      <c r="U56" s="43" t="s">
+      <c r="S56" s="48"/>
+      <c r="U56" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="V56" s="46"/>
-      <c r="W56" s="46" t="s">
+      <c r="V56" s="48"/>
+      <c r="W56" s="48" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="57" s="41" customFormat="1" spans="7:23">
-      <c r="G57" s="48">
+    <row r="57" s="43" customFormat="1" spans="7:23">
+      <c r="G57" s="50">
         <v>1</v>
       </c>
-      <c r="H57" s="46" t="s">
+      <c r="H57" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="R57" s="48">
+      <c r="R57" s="50">
         <v>1</v>
       </c>
-      <c r="S57" s="46" t="s">
+      <c r="S57" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="U57" s="46"/>
-      <c r="V57" s="46"/>
-      <c r="W57" s="46"/>
-    </row>
-    <row r="58" s="41" customFormat="1" spans="7:23">
-      <c r="G58" s="48">
+      <c r="U57" s="48"/>
+      <c r="V57" s="48"/>
+      <c r="W57" s="48"/>
+    </row>
+    <row r="58" s="43" customFormat="1" spans="7:23">
+      <c r="G58" s="50">
         <v>2</v>
       </c>
-      <c r="H58" s="46" t="s">
+      <c r="H58" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="R58" s="48">
+      <c r="R58" s="50">
         <v>2</v>
       </c>
-      <c r="S58" s="46" t="s">
+      <c r="S58" s="48" t="s">
         <v>247</v>
       </c>
-      <c r="U58" s="46"/>
-      <c r="V58" s="46"/>
-      <c r="W58" s="46"/>
-    </row>
-    <row r="59" s="41" customFormat="1" spans="7:23">
-      <c r="G59" s="48">
+      <c r="U58" s="48"/>
+      <c r="V58" s="48"/>
+      <c r="W58" s="48"/>
+    </row>
+    <row r="59" s="43" customFormat="1" spans="7:23">
+      <c r="G59" s="50">
         <v>3</v>
       </c>
-      <c r="H59" s="46" t="s">
+      <c r="H59" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="R59" s="48">
+      <c r="R59" s="50">
         <v>3</v>
       </c>
-      <c r="S59" s="59" t="s">
+      <c r="S59" s="61" t="s">
         <v>249</v>
       </c>
-      <c r="U59" s="60" t="s">
+      <c r="U59" s="62" t="s">
         <v>250</v>
       </c>
-      <c r="V59" s="59"/>
-      <c r="W59" s="60" t="s">
+      <c r="V59" s="61"/>
+      <c r="W59" s="62" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="60" s="41" customFormat="1" spans="7:23">
-      <c r="G60" s="48">
+    <row r="60" s="43" customFormat="1" spans="7:23">
+      <c r="G60" s="50">
         <v>4</v>
       </c>
-      <c r="H60" s="46" t="s">
+      <c r="H60" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="R60" s="48">
+      <c r="R60" s="50">
         <v>4</v>
       </c>
-      <c r="S60" s="46" t="s">
+      <c r="S60" s="48" t="s">
         <v>252</v>
       </c>
-      <c r="U60" s="46"/>
-      <c r="V60" s="46"/>
-      <c r="W60" s="46"/>
-    </row>
-    <row r="61" s="41" customFormat="1" spans="7:23">
-      <c r="G61" s="48">
+      <c r="U60" s="48"/>
+      <c r="V60" s="48"/>
+      <c r="W60" s="48"/>
+    </row>
+    <row r="61" s="43" customFormat="1" spans="7:23">
+      <c r="G61" s="50">
         <v>5</v>
       </c>
-      <c r="H61" s="46" t="s">
+      <c r="H61" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="R61" s="48">
+      <c r="R61" s="50">
         <v>5</v>
       </c>
-      <c r="S61" s="61" t="s">
+      <c r="S61" s="63" t="s">
         <v>254</v>
       </c>
-      <c r="U61" s="62" t="s">
+      <c r="U61" s="64" t="s">
         <v>255</v>
       </c>
-      <c r="V61" s="61"/>
-      <c r="W61" s="62" t="s">
+      <c r="V61" s="63"/>
+      <c r="W61" s="64" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="62" s="41" customFormat="1" spans="7:23">
-      <c r="G62" s="48">
+    <row r="62" s="43" customFormat="1" spans="7:23">
+      <c r="G62" s="50">
         <v>6</v>
       </c>
-      <c r="H62" s="46" t="s">
+      <c r="H62" s="48" t="s">
         <v>256</v>
       </c>
-      <c r="R62" s="48">
+      <c r="R62" s="50">
         <v>6</v>
       </c>
-      <c r="S62" s="46" t="s">
+      <c r="S62" s="48" t="s">
         <v>257</v>
       </c>
-      <c r="U62" s="46"/>
-      <c r="V62" s="46"/>
-      <c r="W62" s="46"/>
-    </row>
-    <row r="63" s="41" customFormat="1" spans="7:23">
-      <c r="G63" s="48">
+      <c r="U62" s="48"/>
+      <c r="V62" s="48"/>
+      <c r="W62" s="48"/>
+    </row>
+    <row r="63" s="43" customFormat="1" spans="7:23">
+      <c r="G63" s="50">
         <v>7</v>
       </c>
-      <c r="H63" s="46" t="s">
+      <c r="H63" s="48" t="s">
         <v>258</v>
       </c>
-      <c r="R63" s="48">
+      <c r="R63" s="50">
         <v>7</v>
       </c>
-      <c r="S63" s="63" t="s">
+      <c r="S63" s="65" t="s">
         <v>259</v>
       </c>
-      <c r="U63" s="64" t="s">
+      <c r="U63" s="66" t="s">
         <v>260</v>
       </c>
-      <c r="V63" s="63"/>
-      <c r="W63" s="64" t="s">
+      <c r="V63" s="65"/>
+      <c r="W63" s="66" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="64" spans="7:23">
-      <c r="G64" s="48">
+      <c r="G64" s="50">
         <v>8</v>
       </c>
-      <c r="H64" s="46" t="s">
+      <c r="H64" s="48" t="s">
         <v>261</v>
       </c>
-      <c r="R64" s="48">
+      <c r="R64" s="50">
         <v>8</v>
       </c>
-      <c r="S64" s="65" t="s">
+      <c r="S64" s="67" t="s">
         <v>262</v>
       </c>
-      <c r="U64" s="66" t="s">
+      <c r="U64" s="68" t="s">
         <v>263</v>
       </c>
-      <c r="V64" s="65"/>
-      <c r="W64" s="66" t="s">
+      <c r="V64" s="67"/>
+      <c r="W64" s="68" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7279,7 +7304,7 @@
   <dimension ref="B1:AH41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X37" sqref="X37"/>
+      <selection activeCell="AE23" sqref="AE23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7343,10 +7368,10 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
-      <c r="AD3" s="36" t="s">
+      <c r="AD3" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="AE3" s="36" t="s">
+      <c r="AE3" s="38" t="s">
         <v>268</v>
       </c>
     </row>
@@ -7408,10 +7433,10 @@
       <c r="T4" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="AD4" s="36" t="s">
+      <c r="AD4" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="AE4" s="36" t="s">
+      <c r="AE4" s="38" t="s">
         <v>289</v>
       </c>
     </row>
@@ -7473,10 +7498,10 @@
       <c r="T5" s="6">
         <v>17</v>
       </c>
-      <c r="AD5" s="36" t="s">
+      <c r="AD5" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="AE5" s="36" t="s">
+      <c r="AE5" s="38" t="s">
         <v>292</v>
       </c>
     </row>
@@ -7538,10 +7563,10 @@
       <c r="T6" s="3">
         <v>17</v>
       </c>
-      <c r="AD6" s="36" t="s">
+      <c r="AD6" s="38" t="s">
         <v>294</v>
       </c>
-      <c r="AE6" s="36" t="s">
+      <c r="AE6" s="38" t="s">
         <v>295</v>
       </c>
     </row>
@@ -7589,14 +7614,14 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="AF8" s="37"/>
-      <c r="AG8" s="40"/>
-      <c r="AH8" s="37"/>
+      <c r="AF8" s="39"/>
+      <c r="AG8" s="42"/>
+      <c r="AH8" s="39"/>
     </row>
     <row r="9" spans="32:34">
-      <c r="AF9" s="37"/>
-      <c r="AG9" s="40"/>
-      <c r="AH9" s="40"/>
+      <c r="AF9" s="39"/>
+      <c r="AG9" s="42"/>
+      <c r="AH9" s="42"/>
     </row>
     <row r="10" spans="2:31">
       <c r="B10" s="10" t="s">
@@ -7625,11 +7650,11 @@
       <c r="W10" s="11"/>
       <c r="X10" s="11"/>
       <c r="Y10" s="11"/>
-      <c r="Z10" s="28"/>
-      <c r="AD10" s="36" t="s">
+      <c r="Z10" s="29"/>
+      <c r="AD10" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="AE10" s="36"/>
+      <c r="AE10" s="38"/>
     </row>
     <row r="11" spans="2:31">
       <c r="B11" s="3" t="s">
@@ -7707,10 +7732,10 @@
       <c r="Z11" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="AD11" s="36" t="s">
+      <c r="AD11" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="AE11" s="38" t="s">
+      <c r="AE11" s="40" t="s">
         <v>324</v>
       </c>
     </row>
@@ -7790,8 +7815,12 @@
       <c r="Z12" s="4">
         <v>41</v>
       </c>
-      <c r="AD12" s="36"/>
-      <c r="AE12" s="39"/>
+      <c r="AD12" s="38" t="s">
+        <v>325</v>
+      </c>
+      <c r="AE12" s="41" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="13" spans="2:31">
       <c r="B13" s="3" t="s">
@@ -7869,12 +7898,12 @@
       <c r="Z13" s="3">
         <v>41</v>
       </c>
-      <c r="AD13" s="36"/>
-      <c r="AE13" s="36"/>
+      <c r="AD13" s="38"/>
+      <c r="AE13" s="38"/>
     </row>
     <row r="14" spans="2:31">
       <c r="B14" s="4" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C14" s="4">
         <v>0</v>
@@ -7948,12 +7977,12 @@
       <c r="Z14" s="4">
         <v>23</v>
       </c>
-      <c r="AD14" s="36"/>
-      <c r="AE14" s="36"/>
+      <c r="AD14" s="38"/>
+      <c r="AE14" s="38"/>
     </row>
     <row r="15" spans="2:26">
       <c r="B15" s="3" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -7991,40 +8020,40 @@
       <c r="N15" s="14">
         <v>11</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="28">
         <v>12</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="28">
         <v>13</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15" s="28">
         <v>14</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15" s="28">
         <v>15</v>
       </c>
-      <c r="S15" s="3">
+      <c r="S15" s="28">
         <v>16</v>
       </c>
-      <c r="T15" s="3">
+      <c r="T15" s="28">
         <v>17</v>
       </c>
-      <c r="U15" s="3">
+      <c r="U15" s="28">
         <v>18</v>
       </c>
-      <c r="V15" s="3">
+      <c r="V15" s="28">
         <v>19</v>
       </c>
-      <c r="W15" s="3">
+      <c r="W15" s="28">
         <v>20</v>
       </c>
-      <c r="X15" s="3">
+      <c r="X15" s="28">
         <v>21</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="Y15" s="28">
         <v>22</v>
       </c>
-      <c r="Z15" s="3">
+      <c r="Z15" s="28">
         <v>23</v>
       </c>
     </row>
@@ -8058,16 +8087,16 @@
       <c r="Z16" s="15"/>
     </row>
     <row r="17" spans="30:31">
-      <c r="AD17" s="36"/>
-      <c r="AE17" s="36"/>
+      <c r="AD17" s="38"/>
+      <c r="AE17" s="38"/>
     </row>
     <row r="18" spans="30:31">
-      <c r="AD18" s="36"/>
-      <c r="AE18" s="36"/>
+      <c r="AD18" s="38"/>
+      <c r="AE18" s="38"/>
     </row>
     <row r="19" spans="2:31">
       <c r="B19" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -8075,23 +8104,23 @@
       <c r="F19" s="2"/>
       <c r="G19" s="16"/>
       <c r="H19" s="17" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
-      <c r="N19" s="28"/>
+      <c r="N19" s="29"/>
       <c r="P19" s="17" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
-      <c r="T19" s="28"/>
+      <c r="T19" s="29"/>
       <c r="V19" s="2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
@@ -8099,54 +8128,54 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
-      <c r="AC19" s="40"/>
-      <c r="AD19" s="36"/>
-      <c r="AE19" s="36"/>
+      <c r="AC19" s="42"/>
+      <c r="AD19" s="38"/>
+      <c r="AE19" s="38"/>
     </row>
     <row r="20" spans="2:29">
       <c r="B20" s="3" t="s">
         <v>269</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
       <c r="K20" s="3" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="P20" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="31"/>
       <c r="S20" s="3" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="V20" s="3" t="s">
         <v>269</v>
@@ -8154,16 +8183,16 @@
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="AA20" s="3" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="AB20" s="3" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="AC20" s="23"/>
     </row>
@@ -8185,7 +8214,7 @@
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="21" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="I21" s="26"/>
       <c r="J21" s="27"/>
@@ -8195,10 +8224,10 @@
       <c r="L21" s="4">
         <v>29</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="32">
         <v>30</v>
       </c>
-      <c r="N21" s="4">
+      <c r="N21" s="32">
         <v>31</v>
       </c>
       <c r="P21" s="21" t="s">
@@ -8249,27 +8278,27 @@
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="19" t="s">
-        <v>326</v>
-      </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="30"/>
+        <v>328</v>
+      </c>
+      <c r="I22" s="30"/>
+      <c r="J22" s="31"/>
       <c r="K22" s="3">
         <v>28</v>
       </c>
       <c r="L22" s="3">
         <v>29</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22" s="32">
         <v>30</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22" s="32">
         <v>31</v>
       </c>
       <c r="P22" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="31"/>
       <c r="S22" s="3">
         <v>46</v>
       </c>
@@ -8277,7 +8306,7 @@
         <v>47</v>
       </c>
       <c r="V22" s="3" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
@@ -8297,7 +8326,7 @@
     </row>
     <row r="23" spans="2:28">
       <c r="B23" s="4" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C23" s="4">
         <v>24</v>
@@ -8313,7 +8342,7 @@
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="21" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="I23" s="26"/>
       <c r="J23" s="27"/>
@@ -8323,14 +8352,14 @@
       <c r="L23" s="4">
         <v>1</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23" s="32">
         <v>2</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N23" s="32">
         <v>3</v>
       </c>
       <c r="P23" s="21" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="Q23" s="26"/>
       <c r="R23" s="27"/>
@@ -8352,7 +8381,7 @@
     </row>
     <row r="24" spans="2:20">
       <c r="B24" s="3" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C24" s="3">
         <v>24</v>
@@ -8406,12 +8435,12 @@
     </row>
     <row r="28" spans="2:16">
       <c r="B28" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -8425,54 +8454,54 @@
         <v>269</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="K29" s="29"/>
-      <c r="L29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="31"/>
       <c r="M29" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="2:16">
       <c r="B30" s="25" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="J30" s="33" t="s">
         <v>358</v>
       </c>
-      <c r="J30" s="31" t="s">
-        <v>356</v>
-      </c>
-      <c r="K30" s="32"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="34" t="s">
+      <c r="K30" s="34"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="36" t="s">
         <v>254</v>
       </c>
-      <c r="N30" s="34" t="s">
+      <c r="N30" s="36" t="s">
         <v>249</v>
       </c>
-      <c r="O30" s="34" t="s">
+      <c r="O30" s="36" t="s">
         <v>259</v>
       </c>
-      <c r="P30" s="34" t="s">
+      <c r="P30" s="36" t="s">
         <v>262</v>
       </c>
     </row>
@@ -8482,11 +8511,11 @@
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
-      <c r="J31" s="35" t="s">
+      <c r="J31" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
@@ -8494,14 +8523,14 @@
     </row>
     <row r="33" spans="2:16">
       <c r="B33" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -8515,66 +8544,66 @@
         <v>269</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="J34" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="K34" s="29"/>
-      <c r="L34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="31"/>
       <c r="M34" s="3" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="35" spans="2:16">
       <c r="B35" s="4" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="J35" s="31" t="s">
-        <v>356</v>
-      </c>
-      <c r="K35" s="32"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="34" t="s">
-        <v>373</v>
-      </c>
-      <c r="N35" s="34" t="s">
         <v>374</v>
       </c>
-      <c r="O35" s="34" t="s">
+      <c r="J35" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="K35" s="34"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="36" t="s">
         <v>375</v>
       </c>
-      <c r="P35" s="34" t="s">
+      <c r="N35" s="36" t="s">
+        <v>376</v>
+      </c>
+      <c r="O35" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="P35" s="36" t="s">
         <v>120</v>
       </c>
     </row>
@@ -8586,11 +8615,11 @@
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
-      <c r="J36" s="35" t="s">
+      <c r="J36" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="K36" s="35"/>
-      <c r="L36" s="35"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
@@ -8598,7 +8627,7 @@
     </row>
     <row r="38" spans="2:20">
       <c r="B38" s="17" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -8617,69 +8646,69 @@
       <c r="Q38" s="11"/>
       <c r="R38" s="11"/>
       <c r="S38" s="11"/>
-      <c r="T38" s="28"/>
+      <c r="T38" s="29"/>
     </row>
     <row r="39" spans="2:20">
       <c r="B39" s="3" t="s">
         <v>269</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>384</v>
-      </c>
-      <c r="K39" s="30"/>
+        <v>386</v>
+      </c>
+      <c r="K39" s="31"/>
       <c r="L39" s="19" t="s">
-        <v>385</v>
-      </c>
-      <c r="M39" s="30"/>
+        <v>387</v>
+      </c>
+      <c r="M39" s="31"/>
       <c r="N39" s="3" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="T39" s="3" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="40" spans="2:20">
       <c r="B40" s="4" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>20</v>
@@ -8692,7 +8721,7 @@
       <c r="H40" s="26"/>
       <c r="I40" s="27"/>
       <c r="J40" s="21" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="K40" s="27"/>
       <c r="L40" s="21" t="s">

</xml_diff>

<commit_message>
add some sample projects
</commit_message>
<xml_diff>
--- a/MIC7001/说明书/MIC7001-A3端口说明.V5.202012.1.xlsx
+++ b/MIC7001/说明书/MIC7001-A3端口说明.V5.202012.1.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="按端子号排序" sheetId="1" r:id="rId1"/>
     <sheet name="按功能分组" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterate="1" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="397">
-  <si>
-    <t>IMC7001-A3 插座C（左）V5.191031</t>
-  </si>
-  <si>
-    <t>IMC7001-A3 插座D（右）V5.191031</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="398">
+  <si>
+    <t>IMC7001-A3 插座C（左）V5.201028</t>
+  </si>
+  <si>
+    <t>IMC7001-A3 插座D（右）V5.201028</t>
   </si>
   <si>
     <t>管脚</t>
@@ -627,6 +627,9 @@
   </si>
   <si>
     <t>DI-17</t>
+  </si>
+  <si>
+    <t>仅支持电流输入</t>
   </si>
   <si>
     <t>17:</t>
@@ -1535,8 +1538,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1599,6 +1602,51 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -1607,9 +1655,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1624,66 +1679,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1699,7 +1695,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1713,9 +1709,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1723,21 +1741,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1819,7 +1822,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1831,7 +1846,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1843,49 +1972,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1897,97 +1990,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2104,30 +2107,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -2152,6 +2131,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -2162,17 +2165,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2195,8 +2187,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2208,145 +2211,145 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3170,7 +3173,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="4072255" y="6419850"/>
-          <a:ext cx="4404360" cy="3660140"/>
+          <a:ext cx="4483100" cy="3660140"/>
           <a:chOff x="4383" y="2780"/>
           <a:chExt cx="6834" cy="5764"/>
         </a:xfrm>
@@ -5290,7 +5293,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>479425</xdr:colOff>
+      <xdr:colOff>400685</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>78740</xdr:rowOff>
     </xdr:to>
@@ -5582,8 +5585,8 @@
   <sheetPr/>
   <dimension ref="B2:W64"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:V2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5598,7 +5601,7 @@
     <col min="8" max="8" width="8.69166666666667" style="43" customWidth="1"/>
     <col min="9" max="9" width="9.34166666666667" style="43" customWidth="1"/>
     <col min="10" max="10" width="9" style="43"/>
-    <col min="11" max="11" width="10.7333333333333" style="43" customWidth="1"/>
+    <col min="11" max="11" width="11.7666666666667" style="43" customWidth="1"/>
     <col min="12" max="12" width="5.20833333333333" style="43" customWidth="1"/>
     <col min="13" max="13" width="4.89166666666667" style="43" customWidth="1"/>
     <col min="14" max="14" width="8.04166666666667" style="43" customWidth="1"/>
@@ -5609,7 +5612,7 @@
     <col min="19" max="19" width="8.69166666666667" style="43" customWidth="1"/>
     <col min="20" max="20" width="8.25833333333333" style="43" customWidth="1"/>
     <col min="21" max="21" width="7.825" style="43" customWidth="1"/>
-    <col min="22" max="22" width="10.5833333333333" style="43" customWidth="1"/>
+    <col min="22" max="22" width="12.9416666666667" style="43" customWidth="1"/>
     <col min="23" max="23" width="9" style="43"/>
     <col min="24" max="24" width="5.975" style="43" customWidth="1"/>
     <col min="25" max="16384" width="9" style="43"/>
@@ -6328,19 +6331,19 @@
       <c r="R19" s="48"/>
       <c r="S19" s="48"/>
       <c r="T19" s="48"/>
-      <c r="V19" s="48" t="s">
-        <v>125</v>
+      <c r="V19" s="45" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="20" s="43" customFormat="1" spans="2:22">
       <c r="B20" s="48" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D20" s="48" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="48"/>
@@ -6348,35 +6351,35 @@
       <c r="H20" s="48"/>
       <c r="I20" s="48"/>
       <c r="J20" s="48"/>
-      <c r="K20" s="48" t="s">
-        <v>125</v>
+      <c r="K20" s="45" t="s">
+        <v>128</v>
       </c>
       <c r="M20" s="48" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N20" s="48" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="O20" s="48" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="R20" s="48"/>
       <c r="S20" s="48"/>
       <c r="T20" s="48"/>
       <c r="U20" s="48"/>
-      <c r="V20" s="48" t="s">
-        <v>125</v>
+      <c r="V20" s="45" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="21" s="43" customFormat="1" spans="2:22">
       <c r="B21" s="48" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48"/>
@@ -6386,13 +6389,13 @@
       <c r="J21" s="48"/>
       <c r="K21" s="48"/>
       <c r="M21" s="48" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N21" s="48" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O21" s="48" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P21" s="48"/>
       <c r="Q21" s="48"/>
@@ -6404,13 +6407,13 @@
     </row>
     <row r="22" s="43" customFormat="1" spans="2:22">
       <c r="B22" s="48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D22" s="48" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E22" s="48"/>
       <c r="G22" s="48"/>
@@ -6419,13 +6422,13 @@
       <c r="J22" s="48"/>
       <c r="K22" s="48"/>
       <c r="M22" s="48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N22" s="48" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O22" s="48" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="P22" s="48"/>
       <c r="Q22" s="48"/>
@@ -6433,19 +6436,19 @@
       <c r="S22" s="48"/>
       <c r="T22" s="48"/>
       <c r="U22" s="48"/>
-      <c r="V22" s="48" t="s">
-        <v>125</v>
+      <c r="V22" s="45" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="23" s="43" customFormat="1" spans="2:22">
       <c r="B23" s="48" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="48"/>
@@ -6454,13 +6457,13 @@
       <c r="I23" s="48"/>
       <c r="K23" s="48"/>
       <c r="M23" s="48" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N23" s="48" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O23" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P23" s="48"/>
       <c r="Q23" s="48"/>
@@ -6468,13 +6471,13 @@
       <c r="S23" s="48"/>
       <c r="T23" s="48"/>
       <c r="U23" s="48"/>
-      <c r="V23" s="48" t="s">
-        <v>125</v>
+      <c r="V23" s="45" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="24" s="43" customFormat="1" spans="2:22">
       <c r="B24" s="48" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C24" s="48"/>
       <c r="F24" s="48"/>
@@ -6488,14 +6491,14 @@
         <v>121</v>
       </c>
       <c r="M24" s="48" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N24" s="48"/>
       <c r="O24" s="48" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="P24" s="48" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="Q24" s="48"/>
       <c r="R24" s="48"/>
@@ -6506,16 +6509,16 @@
     </row>
     <row r="25" s="43" customFormat="1" spans="2:22">
       <c r="B25" s="48" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F25" s="48" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G25" s="48"/>
       <c r="H25" s="48"/>
@@ -6523,14 +6526,14 @@
       <c r="J25" s="48"/>
       <c r="K25" s="48"/>
       <c r="M25" s="48" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="N25" s="48"/>
       <c r="O25" s="48" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="P25" s="48" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Q25" s="48"/>
       <c r="R25" s="48"/>
@@ -6541,21 +6544,21 @@
     </row>
     <row r="26" s="43" customFormat="1" spans="2:22">
       <c r="B26" s="48" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E26" s="48"/>
       <c r="F26" s="48"/>
       <c r="G26" s="48" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H26" s="48" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I26" s="48"/>
       <c r="J26" s="48"/>
@@ -6563,21 +6566,21 @@
         <v>110</v>
       </c>
       <c r="M26" s="48" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N26" s="48" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="O26" s="48" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P26" s="48"/>
       <c r="Q26" s="48"/>
       <c r="R26" s="48" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S26" s="48" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T26" s="48"/>
       <c r="U26" s="48"/>
@@ -6585,41 +6588,41 @@
     </row>
     <row r="27" s="43" customFormat="1" spans="2:22">
       <c r="B27" s="48" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E27" s="48"/>
       <c r="F27" s="48"/>
       <c r="G27" s="48" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H27" s="48" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I27" s="48"/>
       <c r="J27" s="48"/>
       <c r="K27" s="48"/>
       <c r="M27" s="48" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N27" s="48" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="O27" s="48" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="P27" s="48"/>
       <c r="Q27" s="48"/>
       <c r="R27" s="48" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S27" s="48" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T27" s="48"/>
       <c r="U27" s="48"/>
@@ -6629,47 +6632,47 @@
     </row>
     <row r="28" s="43" customFormat="1" spans="2:22">
       <c r="B28" s="48" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E28" s="48"/>
       <c r="F28" s="48"/>
       <c r="G28" s="48" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H28" s="48" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I28" s="48"/>
       <c r="J28" s="48"/>
       <c r="K28" s="48"/>
       <c r="M28" s="48" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="N28" s="48"/>
       <c r="O28" s="48"/>
       <c r="P28" s="48"/>
       <c r="Q28" s="48"/>
       <c r="R28" s="48" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="S28" s="48" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="T28" s="48" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U28" s="48"/>
       <c r="V28" s="48"/>
     </row>
     <row r="29" s="43" customFormat="1" spans="2:22">
       <c r="B29" s="48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C29" s="48"/>
       <c r="D29" s="48"/>
@@ -6679,33 +6682,33 @@
       <c r="H29" s="48"/>
       <c r="I29" s="48"/>
       <c r="J29" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="K29" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="M29" s="48" t="s">
         <v>184</v>
-      </c>
-      <c r="K29" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="M29" s="48" t="s">
-        <v>183</v>
       </c>
       <c r="N29" s="48"/>
       <c r="O29" s="48"/>
       <c r="P29" s="48"/>
       <c r="Q29" s="48"/>
       <c r="R29" s="48" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S29" s="48" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="T29" s="48" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="U29" s="48"/>
       <c r="V29" s="48"/>
     </row>
     <row r="30" s="43" customFormat="1" spans="2:22">
       <c r="B30" s="48" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C30" s="48"/>
       <c r="D30" s="48"/>
@@ -6721,7 +6724,7 @@
         <v>121</v>
       </c>
       <c r="M30" s="48" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N30" s="48"/>
       <c r="O30" s="48"/>
@@ -6739,13 +6742,13 @@
     </row>
     <row r="31" s="43" customFormat="1" spans="2:22">
       <c r="B31" s="48" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E31" s="48"/>
       <c r="F31" s="48"/>
@@ -6754,16 +6757,16 @@
       <c r="I31" s="48"/>
       <c r="J31" s="48"/>
       <c r="K31" s="45" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="M31" s="48" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N31" s="48" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O31" s="48" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="P31" s="48"/>
       <c r="Q31" s="48"/>
@@ -6771,19 +6774,19 @@
       <c r="S31" s="48"/>
       <c r="T31" s="48"/>
       <c r="U31" s="48"/>
-      <c r="V31" s="48" t="s">
-        <v>125</v>
+      <c r="V31" s="45" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="32" s="43" customFormat="1" spans="2:22">
       <c r="B32" s="48" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E32" s="48"/>
       <c r="F32" s="48"/>
@@ -6793,13 +6796,13 @@
       <c r="J32" s="48"/>
       <c r="K32" s="48"/>
       <c r="M32" s="48" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="N32" s="48" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="O32" s="48" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="P32" s="48"/>
       <c r="Q32" s="48"/>
@@ -6807,19 +6810,19 @@
       <c r="S32" s="48"/>
       <c r="T32" s="48"/>
       <c r="U32" s="48"/>
-      <c r="V32" s="48" t="s">
-        <v>125</v>
+      <c r="V32" s="45" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="33" s="43" customFormat="1" spans="2:22">
       <c r="B33" s="48" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E33" s="48"/>
       <c r="F33" s="48"/>
@@ -6829,13 +6832,13 @@
       <c r="J33" s="48"/>
       <c r="K33" s="48"/>
       <c r="M33" s="48" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="N33" s="48" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O33" s="48" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="P33" s="48"/>
       <c r="Q33" s="48"/>
@@ -6843,19 +6846,19 @@
       <c r="S33" s="48"/>
       <c r="T33" s="48"/>
       <c r="U33" s="48"/>
-      <c r="V33" s="48" t="s">
-        <v>125</v>
+      <c r="V33" s="45" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34" s="43" customFormat="1" spans="2:22">
       <c r="B34" s="48" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E34" s="48"/>
       <c r="F34" s="48"/>
@@ -6865,13 +6868,13 @@
       <c r="J34" s="48"/>
       <c r="K34" s="48"/>
       <c r="M34" s="48" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N34" s="48" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O34" s="48" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="P34" s="48"/>
       <c r="Q34" s="48"/>
@@ -6879,13 +6882,13 @@
       <c r="S34" s="48"/>
       <c r="T34" s="48"/>
       <c r="U34" s="48"/>
-      <c r="V34" s="48" t="s">
-        <v>125</v>
+      <c r="V34" s="45" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="35" s="43" customFormat="1" spans="2:22">
       <c r="B35" s="48" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C35" s="48"/>
       <c r="D35" s="48"/>
@@ -6901,7 +6904,7 @@
         <v>121</v>
       </c>
       <c r="M35" s="48" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="P35" s="48"/>
       <c r="Q35" s="48"/>
@@ -6917,25 +6920,25 @@
     </row>
     <row r="36" s="43" customFormat="1" spans="2:22">
       <c r="B36" s="48" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C36" s="48"/>
       <c r="D36" s="48"/>
       <c r="E36" s="48"/>
       <c r="F36" s="48"/>
       <c r="G36" s="48" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H36" s="48" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I36" s="48" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J36" s="48"/>
       <c r="K36" s="48"/>
       <c r="M36" s="48" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N36" s="48"/>
       <c r="O36" s="48"/>
@@ -6945,47 +6948,47 @@
       <c r="S36" s="48"/>
       <c r="T36" s="48"/>
       <c r="U36" s="48" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="V36" s="45" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" s="43" customFormat="1" spans="2:22">
       <c r="B37" s="48" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C37" s="48"/>
       <c r="D37" s="48"/>
       <c r="E37" s="48"/>
       <c r="F37" s="48"/>
       <c r="G37" s="48" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H37" s="48" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I37" s="48" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J37" s="48"/>
       <c r="K37" s="48"/>
       <c r="M37" s="48" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N37" s="48" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="O37" s="48" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="P37" s="48"/>
       <c r="Q37" s="48"/>
       <c r="R37" s="48" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="S37" s="48" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="T37" s="48"/>
       <c r="U37" s="48"/>
@@ -6993,21 +6996,21 @@
     </row>
     <row r="38" s="43" customFormat="1" spans="2:22">
       <c r="B38" s="48" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E38" s="48"/>
       <c r="F38" s="48"/>
       <c r="G38" s="48" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H38" s="48" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I38" s="48"/>
       <c r="J38" s="48"/>
@@ -7015,21 +7018,21 @@
         <v>110</v>
       </c>
       <c r="M38" s="48" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N38" s="48" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="O38" s="48" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="P38" s="48"/>
       <c r="Q38" s="48"/>
       <c r="R38" s="48" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S38" s="48" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="T38" s="48"/>
       <c r="U38" s="48"/>
@@ -7037,7 +7040,7 @@
     </row>
     <row r="40" spans="3:3">
       <c r="C40" s="49" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" s="43" customFormat="1" spans="3:11">
@@ -7045,7 +7048,7 @@
         <v>20</v>
       </c>
       <c r="D41" s="50" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E41" s="50"/>
       <c r="F41" s="50"/>
@@ -7055,10 +7058,10 @@
     </row>
     <row r="42" s="43" customFormat="1" spans="3:11">
       <c r="C42" s="48" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D42" s="51" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E42" s="51"/>
       <c r="F42" s="51"/>
@@ -7068,10 +7071,10 @@
     </row>
     <row r="43" spans="3:7">
       <c r="C43" s="48" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D43" s="51" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E43" s="51"/>
       <c r="F43" s="51"/>
@@ -7085,26 +7088,26 @@
     </row>
     <row r="53" spans="3:3">
       <c r="C53" s="43" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="54" s="43" customFormat="1" spans="7:8">
       <c r="G54" s="55" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H54" s="55"/>
     </row>
     <row r="55" s="43" customFormat="1" spans="7:23">
       <c r="G55" s="56" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H55" s="57"/>
       <c r="R55" s="56" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="S55" s="57"/>
       <c r="U55" s="56" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="V55" s="60"/>
       <c r="W55" s="57"/>
@@ -7119,11 +7122,11 @@
       </c>
       <c r="S56" s="48"/>
       <c r="U56" s="45" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="V56" s="48"/>
       <c r="W56" s="48" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="57" s="43" customFormat="1" spans="7:23">
@@ -7131,7 +7134,7 @@
         <v>1</v>
       </c>
       <c r="H57" s="48" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="R57" s="50">
         <v>1</v>
@@ -7154,7 +7157,7 @@
         <v>2</v>
       </c>
       <c r="S58" s="48" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="U58" s="48"/>
       <c r="V58" s="48"/>
@@ -7165,20 +7168,20 @@
         <v>3</v>
       </c>
       <c r="H59" s="48" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="R59" s="50">
         <v>3</v>
       </c>
       <c r="S59" s="61" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="U59" s="62" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="V59" s="61"/>
       <c r="W59" s="62" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="60" s="43" customFormat="1" spans="7:23">
@@ -7186,13 +7189,13 @@
         <v>4</v>
       </c>
       <c r="H60" s="48" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="R60" s="50">
         <v>4</v>
       </c>
       <c r="S60" s="48" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="U60" s="48"/>
       <c r="V60" s="48"/>
@@ -7203,20 +7206,20 @@
         <v>5</v>
       </c>
       <c r="H61" s="48" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="R61" s="50">
         <v>5</v>
       </c>
       <c r="S61" s="63" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="U61" s="64" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="V61" s="63"/>
       <c r="W61" s="64" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="62" s="43" customFormat="1" spans="7:23">
@@ -7224,13 +7227,13 @@
         <v>6</v>
       </c>
       <c r="H62" s="48" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="R62" s="50">
         <v>6</v>
       </c>
       <c r="S62" s="48" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="U62" s="48"/>
       <c r="V62" s="48"/>
@@ -7241,20 +7244,20 @@
         <v>7</v>
       </c>
       <c r="H63" s="48" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="R63" s="50">
         <v>7</v>
       </c>
       <c r="S63" s="65" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="U63" s="66" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="V63" s="65"/>
       <c r="W63" s="66" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="64" spans="7:23">
@@ -7262,20 +7265,20 @@
         <v>8</v>
       </c>
       <c r="H64" s="48" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="R64" s="50">
         <v>8</v>
       </c>
       <c r="S64" s="67" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="U64" s="68" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="V64" s="67"/>
       <c r="W64" s="68" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -7303,7 +7306,7 @@
   <sheetPr/>
   <dimension ref="B1:AH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AE23" sqref="AE23"/>
     </sheetView>
   </sheetViews>
@@ -7321,7 +7324,7 @@
   <sheetData>
     <row r="1" spans="2:20">
       <c r="B1" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -7343,12 +7346,12 @@
     </row>
     <row r="2" spans="30:30">
       <c r="AD2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="2:31">
       <c r="B3" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -7369,80 +7372,80 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="AD3" s="38" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AE3" s="38" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="2:31">
       <c r="B4" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AD4" s="38" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AE4" s="38" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="2:31">
       <c r="B5" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C5" s="5">
         <v>0</v>
@@ -7499,15 +7502,15 @@
         <v>17</v>
       </c>
       <c r="AD5" s="38" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AE5" s="38" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="2:31">
       <c r="B6" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -7564,15 +7567,15 @@
         <v>17</v>
       </c>
       <c r="AD6" s="38" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AE6" s="38" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="2:20">
       <c r="B7" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
@@ -7595,7 +7598,7 @@
     </row>
     <row r="8" spans="3:34">
       <c r="C8" s="9" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -7625,7 +7628,7 @@
     </row>
     <row r="10" spans="2:31">
       <c r="B10" s="10" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -7652,96 +7655,96 @@
       <c r="Y10" s="11"/>
       <c r="Z10" s="29"/>
       <c r="AD10" s="38" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AE10" s="38"/>
     </row>
     <row r="11" spans="2:31">
       <c r="B11" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="V11" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AD11" s="38" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AE11" s="40" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="2:31">
       <c r="B12" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C12" s="4">
         <v>18</v>
@@ -7816,15 +7819,15 @@
         <v>41</v>
       </c>
       <c r="AD12" s="38" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AE12" s="41" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="2:31">
       <c r="B13" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C13" s="13">
         <v>18</v>
@@ -7903,7 +7906,7 @@
     </row>
     <row r="14" spans="2:31">
       <c r="B14" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C14" s="4">
         <v>0</v>
@@ -7982,7 +7985,7 @@
     </row>
     <row r="15" spans="2:26">
       <c r="B15" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -8059,7 +8062,7 @@
     </row>
     <row r="16" spans="2:26">
       <c r="B16" s="15" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -8096,7 +8099,7 @@
     </row>
     <row r="19" spans="2:31">
       <c r="B19" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -8104,7 +8107,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="16"/>
       <c r="H19" s="17" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -8113,14 +8116,14 @@
       <c r="M19" s="11"/>
       <c r="N19" s="29"/>
       <c r="P19" s="17" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="29"/>
       <c r="V19" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
@@ -8134,71 +8137,71 @@
     </row>
     <row r="20" spans="2:29">
       <c r="B20" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I20" s="30"/>
       <c r="J20" s="31"/>
       <c r="K20" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="Q20" s="30"/>
       <c r="R20" s="31"/>
       <c r="S20" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="V20" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AA20" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AB20" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AC20" s="23"/>
     </row>
     <row r="21" spans="2:29">
       <c r="B21" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C21" s="4">
         <v>42</v>
@@ -8214,7 +8217,7 @@
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="21" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="I21" s="26"/>
       <c r="J21" s="27"/>
@@ -8231,7 +8234,7 @@
         <v>31</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Q21" s="26"/>
       <c r="R21" s="27"/>
@@ -8242,7 +8245,7 @@
         <v>47</v>
       </c>
       <c r="V21" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
@@ -8262,7 +8265,7 @@
     </row>
     <row r="22" spans="2:29">
       <c r="B22" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C22" s="3">
         <v>42</v>
@@ -8278,7 +8281,7 @@
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="19" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="I22" s="30"/>
       <c r="J22" s="31"/>
@@ -8295,7 +8298,7 @@
         <v>31</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="Q22" s="30"/>
       <c r="R22" s="31"/>
@@ -8306,7 +8309,7 @@
         <v>47</v>
       </c>
       <c r="V22" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
@@ -8326,7 +8329,7 @@
     </row>
     <row r="23" spans="2:28">
       <c r="B23" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C23" s="4">
         <v>24</v>
@@ -8342,7 +8345,7 @@
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="21" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="I23" s="26"/>
       <c r="J23" s="27"/>
@@ -8359,7 +8362,7 @@
         <v>3</v>
       </c>
       <c r="P23" s="21" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Q23" s="26"/>
       <c r="R23" s="27"/>
@@ -8370,7 +8373,7 @@
         <v>1</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
@@ -8381,7 +8384,7 @@
     </row>
     <row r="24" spans="2:20">
       <c r="B24" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C24" s="3">
         <v>24</v>
@@ -8397,7 +8400,7 @@
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -8406,7 +8409,7 @@
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
       <c r="P24" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
@@ -8415,7 +8418,7 @@
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -8435,12 +8438,12 @@
     </row>
     <row r="28" spans="2:16">
       <c r="B28" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -8451,68 +8454,68 @@
     </row>
     <row r="29" spans="2:16">
       <c r="B29" s="24" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="K29" s="30"/>
       <c r="L29" s="31"/>
       <c r="M29" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="30" spans="2:16">
       <c r="B30" s="25" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="J30" s="33" t="s">
         <v>359</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="J30" s="33" t="s">
-        <v>358</v>
       </c>
       <c r="K30" s="34"/>
       <c r="L30" s="35"/>
       <c r="M30" s="36" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="N30" s="36" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="O30" s="36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="P30" s="36" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="2:16">
       <c r="B31" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
       <c r="J31" s="37" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K31" s="37"/>
       <c r="L31" s="37"/>
@@ -8523,14 +8526,14 @@
     </row>
     <row r="33" spans="2:16">
       <c r="B33" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -8541,67 +8544,67 @@
     </row>
     <row r="34" spans="2:16">
       <c r="B34" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="J34" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="K34" s="30"/>
       <c r="L34" s="31"/>
       <c r="M34" s="3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="35" spans="2:16">
       <c r="B35" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="J35" s="33" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="K35" s="34"/>
       <c r="L35" s="35"/>
       <c r="M35" s="36" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="N35" s="36" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="O35" s="36" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="P35" s="36" t="s">
         <v>120</v>
@@ -8609,14 +8612,14 @@
     </row>
     <row r="36" spans="2:16">
       <c r="B36" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="J36" s="37" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K36" s="37"/>
       <c r="L36" s="37"/>
@@ -8627,7 +8630,7 @@
     </row>
     <row r="38" spans="2:20">
       <c r="B38" s="17" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -8650,65 +8653,65 @@
     </row>
     <row r="39" spans="2:20">
       <c r="B39" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="K39" s="31"/>
       <c r="L39" s="19" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M39" s="31"/>
       <c r="N39" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="T39" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="40" spans="2:20">
       <c r="B40" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>20</v>
@@ -8721,11 +8724,11 @@
       <c r="H40" s="26"/>
       <c r="I40" s="27"/>
       <c r="J40" s="21" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K40" s="27"/>
       <c r="L40" s="21" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M40" s="27"/>
       <c r="N40" s="21" t="s">
@@ -8740,7 +8743,7 @@
     </row>
     <row r="41" spans="2:20">
       <c r="B41" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="8"/>

</xml_diff>